<commit_message>
V1.00.01 - Documentation for Axis Portal V1
Final documentation for Axis Portal V1 (Release V1.00.00)
</commit_message>
<xml_diff>
--- a/hardware/boards/axis_portal_v1/docs/Documentation.xlsx
+++ b/hardware/boards/axis_portal_v1/docs/Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\josep\goldi2\hardware\boards\axis_portal_v1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C61D0-87C8-4DFF-AA49-8769F2B3D4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F056F9-2D01-44ED-95D5-C80F4539842D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="268">
   <si>
     <t>Signal Name</t>
   </si>
@@ -746,18 +746,12 @@
     <t>REGISTER ADDRESS</t>
   </si>
   <si>
-    <t>REGISTER DATA</t>
-  </si>
-  <si>
     <t>Crossbar Communication Mode:</t>
   </si>
   <si>
     <t>EXTERNAL IO ADDRESS [IO_INDEX + 2]</t>
   </si>
   <si>
-    <t>INTERNAL IO INDEX</t>
-  </si>
-  <si>
     <t>EXTERNAL_IO_ADDRESS[6:0]</t>
   </si>
   <si>
@@ -840,6 +834,15 @@
   </si>
   <si>
     <t>SPI Protocol:</t>
+  </si>
+  <si>
+    <t>REGISTER DATA [MSBF]</t>
+  </si>
+  <si>
+    <t>INTERNAL IO INDEX [MSBF]</t>
+  </si>
+  <si>
+    <t>Multi-word spi transactions follow MSBF order. The second data word is stored in the lower address accessed.  The SPI transfer "ADDRESS[6:0]/DATA_1[7:0]/DATA_2[7:0]" is equivalent to "ADDRESS[6:0] / DATA_1[7:0]   ADDRESS[6:0]-1 / DATA_2[7:0]"</t>
   </si>
 </sst>
 </file>
@@ -948,7 +951,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -1601,12 +1604,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1697,6 +1744,43 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1709,18 +1793,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1739,51 +1811,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1796,12 +1856,87 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1820,105 +1955,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" quotePrefix="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2234,17 +2309,17 @@
       <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="58"/>
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
@@ -3333,90 +3408,90 @@
     </row>
     <row r="54" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="55" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="58"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="69"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="59">
+      <c r="B56" s="70">
         <v>1</v>
       </c>
-      <c r="C56" s="52" t="s">
+      <c r="C56" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="52"/>
-      <c r="E56" s="52"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="52"/>
-      <c r="H56" s="53"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="60"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B57" s="59"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="52"/>
-      <c r="H57" s="53"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="60"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B58" s="60"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="55"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="62"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="41">
         <v>2</v>
       </c>
-      <c r="C59" s="48" t="s">
+      <c r="C59" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="49"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="64"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B60" s="61">
+      <c r="B60" s="72">
         <v>3</v>
       </c>
-      <c r="C60" s="50" t="s">
+      <c r="C60" s="65" t="s">
         <v>226</v>
       </c>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="51"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="65"/>
+      <c r="H60" s="66"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B61" s="59"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="53"/>
+      <c r="B61" s="70"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="60"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B62" s="60"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="55"/>
+      <c r="B62" s="71"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
+      <c r="F62" s="61"/>
+      <c r="G62" s="61"/>
+      <c r="H62" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3442,8 +3517,8 @@
   </sheetPr>
   <dimension ref="B2:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3459,26 +3534,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="12">
         <v>1</v>
       </c>
@@ -3493,10 +3568,10 @@
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>107</v>
       </c>
@@ -3511,10 +3586,10 @@
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="14" t="s">
         <v>206</v>
       </c>
@@ -3529,34 +3604,34 @@
       <c r="M5" s="12"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="80" t="s">
         <v>225</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="31"/>
@@ -3625,7 +3700,7 @@
       <c r="J11" s="27"/>
       <c r="K11" s="26"/>
       <c r="L11" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="M11" s="36" t="s">
         <v>124</v>
@@ -3633,7 +3708,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C12" s="20">
         <v>2</v>
@@ -3644,34 +3719,20 @@
       <c r="E12" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>18</v>
-      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
       <c r="M12" s="37" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C13" s="20">
         <v>3</v>
@@ -3682,15 +3743,29 @@
       <c r="E13" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="M13" s="37" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -3784,19 +3859,19 @@
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L16" s="21" t="s">
         <v>152</v>
@@ -3828,7 +3903,7 @@
         <v>155</v>
       </c>
       <c r="M17" s="37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -3854,7 +3929,7 @@
         <v>155</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -3870,16 +3945,16 @@
       <c r="E19" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="34" t="s">
@@ -3894,16 +3969,16 @@
       <c r="E20" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="72" t="s">
+      <c r="F20" s="76" t="s">
         <v>183</v>
       </c>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="73"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="77"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="34" t="s">
@@ -3918,16 +3993,16 @@
       <c r="E21" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="72" t="s">
+      <c r="F21" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="73"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="77"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
@@ -3942,16 +4017,16 @@
       <c r="E22" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="73"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="77"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
@@ -3992,16 +4067,16 @@
       <c r="E24" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="72" t="s">
+      <c r="F24" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="73"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="77"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="34" t="s">
@@ -4042,16 +4117,16 @@
       <c r="E26" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="73"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="77"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="34" t="s">
@@ -4092,16 +4167,16 @@
       <c r="E28" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="72" t="s">
+      <c r="F28" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="72"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="72"/>
-      <c r="M28" s="73"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="77"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
@@ -4146,16 +4221,16 @@
       <c r="G30" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H30" s="69" t="s">
+      <c r="H30" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="I30" s="104"/>
-      <c r="J30" s="105"/>
-      <c r="K30" s="69" t="s">
+      <c r="I30" s="74"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="L30" s="104"/>
-      <c r="M30" s="104"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="74"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
@@ -4176,16 +4251,16 @@
       <c r="G31" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H31" s="68" t="s">
+      <c r="H31" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68" t="s">
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="L31" s="68"/>
-      <c r="M31" s="69"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="73"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="34" t="s">
@@ -4206,16 +4281,16 @@
       <c r="G32" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H32" s="68" t="s">
+      <c r="H32" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68" t="s">
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="L32" s="68"/>
-      <c r="M32" s="69"/>
+      <c r="L32" s="81"/>
+      <c r="M32" s="73"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="34" t="s">
@@ -4236,22 +4311,22 @@
       <c r="G33" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H33" s="68" t="s">
+      <c r="H33" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68" t="s">
+      <c r="I33" s="81"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="L33" s="68"/>
-      <c r="M33" s="69"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="73"/>
     </row>
     <row r="34" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="C34" s="108">
+      <c r="C34" s="48">
         <v>24</v>
       </c>
       <c r="D34" s="35" t="s">
@@ -4266,26 +4341,22 @@
       <c r="G34" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="82" t="s">
         <v>204</v>
       </c>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70" t="s">
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="L34" s="70"/>
-      <c r="M34" s="71"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="83"/>
     </row>
     <row r="35" spans="2:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-    </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="17"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
@@ -4340,6 +4411,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="K32:M32"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="F22:M22"/>
@@ -4354,14 +4433,6 @@
     <mergeCell ref="F19:M19"/>
     <mergeCell ref="F20:M20"/>
     <mergeCell ref="F21:M21"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="K32:M32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4389,441 +4460,436 @@
       <c r="B2" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="84" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="84" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="84" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="84" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="84" t="s">
         <v>211</v>
       </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
-      <c r="J10" s="78"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="84" t="s">
         <v>215</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="84" t="s">
         <v>216</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="85"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="77" t="s">
-        <v>253</v>
-      </c>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
+      <c r="C13" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C14" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="109"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="109"/>
+      <c r="C14" s="84" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="77" t="s">
-        <v>255</v>
-      </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
+      <c r="C15" s="84" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="85"/>
+      <c r="M15" s="85"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="77" t="s">
-        <v>256</v>
-      </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="109"/>
-      <c r="K16" s="109"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
+      <c r="C16" s="84" t="s">
+        <v>254</v>
+      </c>
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="85"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="84" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="78"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="85"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="85"/>
+      <c r="L17" s="85"/>
+      <c r="M17" s="85"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="84" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="78"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-      <c r="M18" s="78"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="85"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="84" t="s">
         <v>219</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="84" t="s">
         <v>220</v>
       </c>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-      <c r="M20" s="78"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="C21" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" s="84" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="78"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="85"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="C22" s="84" t="s">
         <v>222</v>
       </c>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="85"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" s="84" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C25" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="D23" s="78"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="111" t="s">
-        <v>250</v>
-      </c>
-      <c r="C24" s="77" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="111" t="s">
-        <v>251</v>
-      </c>
-      <c r="C25" s="77" t="s">
-        <v>259</v>
-      </c>
-      <c r="D25" s="78"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78"/>
-      <c r="J25" s="78"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="78"/>
-      <c r="M25" s="78"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C14:M14"/>
-    <mergeCell ref="C16:M16"/>
-    <mergeCell ref="C23:M23"/>
-    <mergeCell ref="C24:M24"/>
-    <mergeCell ref="C25:M25"/>
     <mergeCell ref="C13:M13"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="C3:M3"/>
@@ -4836,6 +4902,11 @@
     <mergeCell ref="C10:M10"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C12:M12"/>
+    <mergeCell ref="C14:M14"/>
+    <mergeCell ref="C16:M16"/>
+    <mergeCell ref="C23:M23"/>
+    <mergeCell ref="C24:M24"/>
+    <mergeCell ref="C25:M25"/>
     <mergeCell ref="C22:M22"/>
     <mergeCell ref="C15:M15"/>
     <mergeCell ref="C17:M17"/>
@@ -4855,10 +4926,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:Q30"/>
+  <dimension ref="B2:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4888,11 +4959,11 @@
       <c r="Q2" s="102"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="98" t="s">
         <v>227</v>
       </c>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="103" t="s">
         <v>229</v>
       </c>
@@ -4911,26 +4982,26 @@
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="99" t="s">
         <v>230</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="90" t="s">
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="92"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="101"/>
     </row>
     <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="45" t="s">
@@ -4986,118 +5057,118 @@
       <c r="B8" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="104" t="s">
         <v>234</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="96" t="s">
-        <v>235</v>
-      </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="95"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="106" t="s">
+        <v>265</v>
+      </c>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="105"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="107"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="43">
         <v>0</v>
       </c>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="108" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="99" t="s">
-        <v>243</v>
-      </c>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="101"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="113"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="113"/>
+      <c r="Q9" s="114"/>
     </row>
     <row r="10" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="42">
         <v>1</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="110" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="83" t="s">
-        <v>244</v>
-      </c>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="84"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="115" t="s">
+        <v>242</v>
+      </c>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="111"/>
+      <c r="N10" s="111"/>
+      <c r="O10" s="111"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="116"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="89" t="s">
-        <v>236</v>
-      </c>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="85" t="s">
-        <v>240</v>
-      </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
+      <c r="B13" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="117" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="117"/>
+      <c r="O13" s="117"/>
+      <c r="P13" s="117"/>
+      <c r="Q13" s="117"/>
     </row>
     <row r="14" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="99" t="s">
         <v>230</v>
       </c>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="90" t="s">
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="99" t="s">
         <v>231</v>
       </c>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="92"/>
+      <c r="K15" s="100"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="101"/>
     </row>
     <row r="16" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="45" t="s">
@@ -5153,199 +5224,233 @@
       <c r="B17" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="C17" s="93" t="s">
-        <v>237</v>
-      </c>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="96" t="s">
-        <v>238</v>
-      </c>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="94"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="95"/>
+      <c r="C17" s="104" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="106" t="s">
+        <v>266</v>
+      </c>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="105"/>
+      <c r="Q17" s="107"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="43">
         <v>0</v>
       </c>
-      <c r="C18" s="97" t="s">
+      <c r="C18" s="108" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" s="109"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="112" t="s">
         <v>239</v>
       </c>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="99" t="s">
-        <v>241</v>
-      </c>
-      <c r="K18" s="100"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="100"/>
-      <c r="N18" s="100"/>
-      <c r="O18" s="100"/>
-      <c r="P18" s="100"/>
-      <c r="Q18" s="101"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="113"/>
+      <c r="N18" s="113"/>
+      <c r="O18" s="113"/>
+      <c r="P18" s="113"/>
+      <c r="Q18" s="114"/>
     </row>
     <row r="19" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="42">
         <v>1</v>
       </c>
-      <c r="C19" s="81" t="s">
-        <v>239</v>
-      </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="83" t="s">
-        <v>242</v>
-      </c>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="84"/>
+      <c r="C19" s="110" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="115" t="s">
+        <v>240</v>
+      </c>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="111"/>
+      <c r="Q19" s="116"/>
     </row>
     <row r="21" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="87"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="87"/>
-      <c r="Q22" s="88"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="119"/>
+      <c r="H22" s="119"/>
+      <c r="I22" s="119"/>
+      <c r="J22" s="119"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="119"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="119"/>
+      <c r="P22" s="119"/>
+      <c r="Q22" s="120"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="59">
+      <c r="B23" s="133">
         <v>1</v>
       </c>
-      <c r="C23" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="53"/>
+      <c r="C23" s="124" t="s">
+        <v>243</v>
+      </c>
+      <c r="D23" s="124"/>
+      <c r="E23" s="124"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="124"/>
+      <c r="H23" s="124"/>
+      <c r="I23" s="124"/>
+      <c r="J23" s="124"/>
+      <c r="K23" s="124"/>
+      <c r="L23" s="124"/>
+      <c r="M23" s="124"/>
+      <c r="N23" s="124"/>
+      <c r="O23" s="124"/>
+      <c r="P23" s="124"/>
+      <c r="Q23" s="125"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="60"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="55"/>
-    </row>
-    <row r="28" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="89" t="s">
-        <v>266</v>
-      </c>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="118" t="s">
+      <c r="B24" s="126"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="127"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="123">
+        <v>2</v>
+      </c>
+      <c r="C25" s="121" t="s">
+        <v>267</v>
+      </c>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="122"/>
+      <c r="Q25" s="128"/>
+    </row>
+    <row r="26" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="129"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="131"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="131"/>
+      <c r="P26" s="131"/>
+      <c r="Q26" s="132"/>
+    </row>
+    <row r="30" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="98" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="49" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" s="88" t="s">
+        <v>259</v>
+      </c>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="90"/>
+      <c r="H31" s="51">
+        <v>1</v>
+      </c>
+      <c r="I31" s="96" t="s">
+        <v>263</v>
+      </c>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="96"/>
+      <c r="N31" s="97"/>
+    </row>
+    <row r="32" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="50" t="s">
         <v>260</v>
       </c>
-      <c r="C29" s="120" t="s">
+      <c r="C32" s="91" t="s">
         <v>261</v>
       </c>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="124">
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="52">
         <v>1</v>
       </c>
-      <c r="I29" s="113" t="s">
-        <v>265</v>
-      </c>
-      <c r="J29" s="113"/>
-      <c r="K29" s="113"/>
-      <c r="L29" s="113"/>
-      <c r="M29" s="113"/>
-      <c r="N29" s="114"/>
-    </row>
-    <row r="30" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="119" t="s">
+      <c r="I32" s="94" t="s">
         <v>262</v>
       </c>
-      <c r="C30" s="122" t="s">
-        <v>263</v>
-      </c>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="125">
-        <v>1</v>
-      </c>
-      <c r="I30" s="116" t="s">
-        <v>264</v>
-      </c>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="117"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="95"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="I30:N30"/>
-    <mergeCell ref="I29:N29"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B6:I6"/>
+  <mergeCells count="31">
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="E4:Q4"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="C8:I8"/>
     <mergeCell ref="J6:Q6"/>
     <mergeCell ref="J8:Q8"/>
@@ -5359,6 +5464,12 @@
     <mergeCell ref="C23:Q24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B22:Q22"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="I32:N32"/>
+    <mergeCell ref="I31:N31"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B6:I6"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="J15:Q15"/>
@@ -5366,6 +5477,8 @@
     <mergeCell ref="J17:Q17"/>
     <mergeCell ref="C18:I18"/>
     <mergeCell ref="J18:Q18"/>
+    <mergeCell ref="C25:Q26"/>
+    <mergeCell ref="B25:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>